<commit_message>
add: notebook 04 for ATD and stack
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/ArabSign Labeled Sentence.xlsx
+++ b/Dataset Excel Sheets/ArabSign Labeled Sentence.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salma\Desktop\Senior Design\CSE 491 - Senior Design II\github\Senior-Design-Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaher.salman\Desktop\LINA JAN 24\Senior II\Senior-Design-Code\Dataset Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6416D8-988B-408E-961D-356790031D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="9420" windowHeight="11040" xr2:uid="{189A1E0C-090A-4C68-8075-4E2BBB4D9E7D}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="9420" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,8 +340,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -707,16 +706,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41C73D6-5046-4311-8732-E7F8853832D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -732,7 +734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -740,7 +742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -748,7 +750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -756,7 +758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -764,7 +766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -772,7 +774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -780,7 +782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -788,7 +790,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -796,7 +798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -804,7 +806,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -812,7 +814,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -820,7 +822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -828,7 +830,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -836,7 +838,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -844,7 +846,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -852,7 +854,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -860,7 +862,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -868,7 +870,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -876,7 +878,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -884,7 +886,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -892,7 +894,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -900,7 +902,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -908,7 +910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -916,7 +918,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -924,7 +926,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -932,7 +934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -940,7 +942,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -948,7 +950,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -956,7 +958,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -964,7 +966,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -972,7 +974,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -980,7 +982,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -988,7 +990,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -996,7 +998,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -1012,7 +1014,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
@@ -1028,7 +1030,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
@@ -1036,7 +1038,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
@@ -1044,7 +1046,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -1060,7 +1062,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
@@ -1068,7 +1070,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
@@ -1092,7 +1094,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1100,7 +1102,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
@@ -1108,7 +1110,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1118,5 +1120,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>